<commit_message>
Added functionality - asking number of seats, available seats, list of people in the openspace
</commit_message>
<xml_diff>
--- a/Updated_seating_plan.xlsx
+++ b/Updated_seating_plan.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nicole</t>
+          <t>Therese</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -472,7 +472,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>Karthika</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -488,7 +488,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Boitumelo</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -504,7 +504,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Andrii</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -520,7 +520,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fatemeh</t>
+          <t>An</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -536,7 +536,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Therese</t>
+          <t>Jessica</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -552,7 +552,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Stef</t>
+          <t>Miro</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Vera</t>
+          <t>Maxim</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -584,7 +584,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Miriam</t>
+          <t>Jean</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -616,7 +616,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Edoardo</t>
+          <t>Miriam</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -632,7 +632,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Nina</t>
+          <t>Olha</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -648,7 +648,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>New Arrival</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -680,7 +680,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Mohamad</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -696,7 +696,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Yassine</t>
+          <t>Edoardo</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -712,7 +712,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Aleksander</t>
+          <t>Celina</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -728,7 +728,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Kevin P</t>
+          <t>new_1</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -744,7 +744,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Miro</t>
+          <t>Elsa</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -760,7 +760,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Manel</t>
+          <t>Kevin J</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Karthika</t>
+          <t>Manel</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -792,7 +792,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Kevin J</t>
+          <t>Aleksander</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -808,7 +808,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Celina</t>
+          <t>Vera</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -824,7 +824,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Olha</t>
+          <t>Oscar</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -840,7 +840,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Patrycja</t>
+          <t>Stef</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -856,7 +856,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Dhanya</t>
+          <t>Kevin P</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -872,7 +872,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Mohamad</t>
+          <t>Fatemeh</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -888,7 +888,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Elsa</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -904,7 +904,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>An</t>
+          <t>Yassine</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -920,7 +920,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Beatriz</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -936,7 +936,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Oscar</t>
+          <t>Nicole</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -952,7 +952,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Boitumelo</t>
+          <t>Patrycja</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -968,7 +968,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Andrii</t>
+          <t>Dhanya</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Nina</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Maxim</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1016,13 +1016,77 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Beatriz</t>
         </is>
       </c>
       <c r="C37" t="n">
         <v>9</v>
       </c>
       <c r="D37" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>10</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>10</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>10</v>
+      </c>
+      <c r="D40" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>10</v>
+      </c>
+      <c r="D41" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>